<commit_message>
added dataset under batch-02
</commit_message>
<xml_diff>
--- a/batch_02/session_01.xlsx
+++ b/batch_02/session_01.xlsx
@@ -12,10 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="demo_sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">demo_sheet!$A$1:$L$21</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>Student ID</t>
   </si>
@@ -228,6 +230,35 @@
   </si>
   <si>
     <t>Agra</t>
+  </si>
+  <si>
+    <t>total
+=H2+I2+J2+K2+L2</t>
+  </si>
+  <si>
+    <t>total
+=sum(starting value:ending value cell id)</t>
+  </si>
+  <si>
+    <t>=J2*K2*L2*M2*N2</t>
+  </si>
+  <si>
+    <t>=PRODUCT(H2:L2)</t>
+  </si>
+  <si>
+    <t>=QUOTIENT(M2,L2)</t>
+  </si>
+  <si>
+    <t>=MOD(M2,L2)</t>
+  </si>
+  <si>
+    <t>=COUNT(start:(end))</t>
+  </si>
+  <si>
+    <t>=COUNTA(start:(end))</t>
+  </si>
+  <si>
+    <t>=AVERAGE(H2:L2)</t>
   </si>
 </sst>
 </file>
@@ -278,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -290,9 +321,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -575,33 +613,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="22.1796875" style="5" customWidth="1"/>
+    <col min="16" max="16" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="12.26953125" customWidth="1"/>
+    <col min="20" max="20" width="13.81640625" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -634,8 +684,35 @@
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -672,8 +749,44 @@
       <c r="L2" s="2">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <f>H2+I2+J2+K2+L2</f>
+        <v>423</v>
+      </c>
+      <c r="N2">
+        <f>SUM(H2:L2)</f>
+        <v>423</v>
+      </c>
+      <c r="O2" s="5">
+        <f>H2*I2*J2*K2*L2</f>
+        <v>4294118400</v>
+      </c>
+      <c r="P2">
+        <f>PRODUCT(H2:L2)</f>
+        <v>4294118400</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>QUOTIENT(M2,L2)</f>
+        <v>4</v>
+      </c>
+      <c r="R2" s="1">
+        <f>MOD(M2,L2)</f>
+        <v>71</v>
+      </c>
+      <c r="S2" s="7">
+        <f>COUNT(O2:O5)</f>
+        <v>4</v>
+      </c>
+      <c r="T2" s="7">
+        <f>COUNTA(B2:B5)</f>
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <f>AVERAGE(H2:L2)</f>
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -710,8 +823,44 @@
       <c r="L3" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <f t="shared" ref="M3:M21" si="0">H3+I3+J3+K3+L3</f>
+        <v>437</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N21" si="1">SUM(H3:L3)</f>
+        <v>437</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O21" si="2">H3*I3*J3*K3*L3</f>
+        <v>5087464200</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P21" si="3">PRODUCT(H3:L3)</f>
+        <v>5087464200</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q21" si="4">QUOTIENT(M3,L3)</f>
+        <v>5</v>
+      </c>
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R21" si="5">MOD(M3,L3)</f>
+        <v>17</v>
+      </c>
+      <c r="S3" s="7">
+        <f t="shared" ref="S3:S21" si="6">COUNT(O3:O6)</f>
+        <v>4</v>
+      </c>
+      <c r="T3" s="7">
+        <f t="shared" ref="T3:T21" si="7">COUNTA(B3:B6)</f>
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U21" si="8">AVERAGE(H3:L3)</f>
+        <v>87.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -748,8 +897,44 @@
       <c r="L4" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>415</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="2"/>
+        <v>3899237760</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>3899237760</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="S4" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T4" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="8"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -786,8 +971,44 @@
       <c r="L5" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>437</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>437</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="2"/>
+        <v>5088763680</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>5088763680</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="S5" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T5" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="8"/>
+        <v>87.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -824,8 +1045,44 @@
       <c r="L6" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>391</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>391</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="2"/>
+        <v>2898062860</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>2898062860</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="5"/>
+        <v>63</v>
+      </c>
+      <c r="S6" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T6" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="8"/>
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -862,8 +1119,44 @@
       <c r="L7" s="2">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>455</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>455</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="2"/>
+        <v>6229102880</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>6229102880</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T7" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="8"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -900,8 +1193,44 @@
       <c r="L8" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>399</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="2"/>
+        <v>3224686080</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>3224686080</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T8" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="8"/>
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -938,8 +1267,44 @@
       <c r="L9" s="2">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>423</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="2"/>
+        <v>4302421200</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>4302421200</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T9" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="8"/>
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -976,8 +1341,44 @@
       <c r="L10" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>406</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="2"/>
+        <v>3526104960</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>3526104960</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="S10" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T10" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="8"/>
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1014,8 +1415,44 @@
       <c r="L11" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>435</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="2"/>
+        <v>4970813760</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>4970813760</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="S11" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T11" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1052,8 +1489,44 @@
       <c r="L12" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>407</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>407</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="2"/>
+        <v>3561143040</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>3561143040</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="5"/>
+        <v>71</v>
+      </c>
+      <c r="S12" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T12" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="8"/>
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1090,8 +1563,44 @@
       <c r="L13" s="2">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="2"/>
+        <v>5269159350</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>5269159350</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="S13" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T13" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="8"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1128,8 +1637,44 @@
       <c r="L14" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>399</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="2"/>
+        <v>3221064000</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>3221064000</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="S14" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T14" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="8"/>
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1166,8 +1711,44 @@
       <c r="L15" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>459</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="2"/>
+        <v>6509166300</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>6509166300</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T15" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="8"/>
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1204,8 +1785,44 @@
       <c r="L16" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>409</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>409</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="2"/>
+        <v>3655108800</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>3655108800</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T16" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="8"/>
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1242,8 +1859,44 @@
       <c r="L17" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>443</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="2"/>
+        <v>5451684480</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>5451684480</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="5"/>
+        <v>83</v>
+      </c>
+      <c r="S17" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T17" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="8"/>
+        <v>88.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1280,8 +1933,44 @@
       <c r="L18" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>392</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>392</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="2"/>
+        <v>2953968000</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>2953968000</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="S18" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T18" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="8"/>
+        <v>78.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1318,8 +2007,44 @@
       <c r="L19" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>433</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>433</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="2"/>
+        <v>4863196800</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>4863196800</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="S19" s="7">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="T19" s="7">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="8"/>
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1356,8 +2081,44 @@
       <c r="L20" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" si="2"/>
+        <v>3687173952</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>3687173952</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="5"/>
+        <v>74</v>
+      </c>
+      <c r="S20" s="7">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T20" s="7">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="8"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1394,9 +2155,458 @@
       <c r="L21" s="2">
         <v>86</v>
       </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>444</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" si="2"/>
+        <v>5513635440</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>5513635440</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T21" s="7">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="8"/>
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="str">
+        <f>demo_sheet!A1</f>
+        <v>Student ID</v>
+      </c>
+      <c r="B1" t="str">
+        <f>demo_sheet!B1</f>
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
+        <f>demo_sheet!D1</f>
+        <v>Gender</v>
+      </c>
+      <c r="D1" t="str">
+        <f>demo_sheet!E1</f>
+        <v>City</v>
+      </c>
+      <c r="E1" t="str">
+        <f>demo_sheet!F1</f>
+        <v>State</v>
+      </c>
+      <c r="F1" t="str">
+        <f>demo_sheet!G1</f>
+        <v>Country</v>
+      </c>
+      <c r="G1" t="str">
+        <f>demo_sheet!H1</f>
+        <v>Mathematics</v>
+      </c>
+      <c r="H1" t="str">
+        <f>demo_sheet!I1</f>
+        <v>Science</v>
+      </c>
+      <c r="I1" t="str">
+        <f>demo_sheet!J1</f>
+        <v>English</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>demo_sheet!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>demo_sheet!B2</f>
+        <v>Aarav Sharma</v>
+      </c>
+      <c r="C2" t="str">
+        <f>demo_sheet!D2</f>
+        <v>Male</v>
+      </c>
+      <c r="D2" t="str">
+        <f>demo_sheet!E2</f>
+        <v>Mumbai</v>
+      </c>
+      <c r="E2" t="str">
+        <f>demo_sheet!F2</f>
+        <v>Maharashtra</v>
+      </c>
+      <c r="F2" t="str">
+        <f>demo_sheet!G2</f>
+        <v>India</v>
+      </c>
+      <c r="G2">
+        <f>demo_sheet!H2</f>
+        <v>85</v>
+      </c>
+      <c r="H2">
+        <f>demo_sheet!I2</f>
+        <v>78</v>
+      </c>
+      <c r="I2">
+        <f>demo_sheet!J2</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>demo_sheet!A3</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>demo_sheet!B3</f>
+        <v>Aanya Patel</v>
+      </c>
+      <c r="C3" t="str">
+        <f>demo_sheet!D3</f>
+        <v>Female</v>
+      </c>
+      <c r="D3" t="str">
+        <f>demo_sheet!E3</f>
+        <v>Delhi</v>
+      </c>
+      <c r="E3" t="str">
+        <f>demo_sheet!F3</f>
+        <v>Delhi</v>
+      </c>
+      <c r="F3" t="str">
+        <f>demo_sheet!G3</f>
+        <v>India</v>
+      </c>
+      <c r="G3">
+        <f>demo_sheet!H3</f>
+        <v>90</v>
+      </c>
+      <c r="H3">
+        <f>demo_sheet!I3</f>
+        <v>85</v>
+      </c>
+      <c r="I3">
+        <f>demo_sheet!J3</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>demo_sheet!A4</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>demo_sheet!B4</f>
+        <v>Aryan Singh</v>
+      </c>
+      <c r="C4" t="str">
+        <f>demo_sheet!D4</f>
+        <v>Male</v>
+      </c>
+      <c r="D4" t="str">
+        <f>demo_sheet!E4</f>
+        <v>Bangalore</v>
+      </c>
+      <c r="E4" t="str">
+        <f>demo_sheet!F4</f>
+        <v>Karnataka</v>
+      </c>
+      <c r="F4" t="str">
+        <f>demo_sheet!G4</f>
+        <v>India</v>
+      </c>
+      <c r="G4">
+        <f>demo_sheet!H4</f>
+        <v>76</v>
+      </c>
+      <c r="H4">
+        <f>demo_sheet!I4</f>
+        <v>82</v>
+      </c>
+      <c r="I4">
+        <f>demo_sheet!J4</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f>demo_sheet!A5</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>demo_sheet!B5</f>
+        <v>Isha Verma</v>
+      </c>
+      <c r="C5" t="str">
+        <f>demo_sheet!D5</f>
+        <v>Female</v>
+      </c>
+      <c r="D5" t="str">
+        <f>demo_sheet!E5</f>
+        <v>Chennai</v>
+      </c>
+      <c r="E5" t="str">
+        <f>demo_sheet!F5</f>
+        <v>Tamil Nadu</v>
+      </c>
+      <c r="F5" t="str">
+        <f>demo_sheet!G5</f>
+        <v>India</v>
+      </c>
+      <c r="G5">
+        <f>demo_sheet!H5</f>
+        <v>88</v>
+      </c>
+      <c r="H5">
+        <f>demo_sheet!I5</f>
+        <v>91</v>
+      </c>
+      <c r="I5">
+        <f>demo_sheet!J5</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f>demo_sheet!A6</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>demo_sheet!B6</f>
+        <v>Vihaan Gupta</v>
+      </c>
+      <c r="C6" t="str">
+        <f>demo_sheet!D6</f>
+        <v>Male</v>
+      </c>
+      <c r="D6" t="str">
+        <f>demo_sheet!E6</f>
+        <v>Hyderabad</v>
+      </c>
+      <c r="E6" t="str">
+        <f>demo_sheet!F6</f>
+        <v>Telangana</v>
+      </c>
+      <c r="F6" t="str">
+        <f>demo_sheet!G6</f>
+        <v>India</v>
+      </c>
+      <c r="G6">
+        <f>demo_sheet!H6</f>
+        <v>70</v>
+      </c>
+      <c r="H6">
+        <f>demo_sheet!I6</f>
+        <v>79</v>
+      </c>
+      <c r="I6">
+        <f>demo_sheet!J6</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f>demo_sheet!A7</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>demo_sheet!B7</f>
+        <v>Saanvi Reddy</v>
+      </c>
+      <c r="C7" t="str">
+        <f>demo_sheet!D7</f>
+        <v>Female</v>
+      </c>
+      <c r="D7" t="str">
+        <f>demo_sheet!E7</f>
+        <v>Pune</v>
+      </c>
+      <c r="E7" t="str">
+        <f>demo_sheet!F7</f>
+        <v>Maharashtra</v>
+      </c>
+      <c r="F7" t="str">
+        <f>demo_sheet!G7</f>
+        <v>India</v>
+      </c>
+      <c r="G7">
+        <f>demo_sheet!H7</f>
+        <v>95</v>
+      </c>
+      <c r="H7">
+        <f>demo_sheet!I7</f>
+        <v>88</v>
+      </c>
+      <c r="I7">
+        <f>demo_sheet!J7</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f>demo_sheet!A8</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>demo_sheet!B8</f>
+        <v>Arjun Kumar</v>
+      </c>
+      <c r="C8" t="str">
+        <f>demo_sheet!D8</f>
+        <v>Male</v>
+      </c>
+      <c r="D8" t="str">
+        <f>demo_sheet!E8</f>
+        <v>Kolkata</v>
+      </c>
+      <c r="E8" t="str">
+        <f>demo_sheet!F8</f>
+        <v>West Bengal</v>
+      </c>
+      <c r="F8" t="str">
+        <f>demo_sheet!G8</f>
+        <v>India</v>
+      </c>
+      <c r="G8">
+        <f>demo_sheet!H8</f>
+        <v>84</v>
+      </c>
+      <c r="H8">
+        <f>demo_sheet!I8</f>
+        <v>76</v>
+      </c>
+      <c r="I8">
+        <f>demo_sheet!J8</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f>demo_sheet!A9</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f>demo_sheet!B9</f>
+        <v>Diya Agarwal</v>
+      </c>
+      <c r="C9" t="str">
+        <f>demo_sheet!D9</f>
+        <v>Female</v>
+      </c>
+      <c r="D9" t="str">
+        <f>demo_sheet!E9</f>
+        <v>Jaipur</v>
+      </c>
+      <c r="E9" t="str">
+        <f>demo_sheet!F9</f>
+        <v>Rajasthan</v>
+      </c>
+      <c r="F9" t="str">
+        <f>demo_sheet!G9</f>
+        <v>India</v>
+      </c>
+      <c r="G9">
+        <f>demo_sheet!H9</f>
+        <v>77</v>
+      </c>
+      <c r="H9">
+        <f>demo_sheet!I9</f>
+        <v>83</v>
+      </c>
+      <c r="I9">
+        <f>demo_sheet!J9</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f>demo_sheet!A10</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f>demo_sheet!B10</f>
+        <v>Kabir Mehta</v>
+      </c>
+      <c r="C10" t="str">
+        <f>demo_sheet!D10</f>
+        <v>Male</v>
+      </c>
+      <c r="D10" t="str">
+        <f>demo_sheet!E10</f>
+        <v>Ahmedabad</v>
+      </c>
+      <c r="E10" t="str">
+        <f>demo_sheet!F10</f>
+        <v>Gujarat</v>
+      </c>
+      <c r="F10" t="str">
+        <f>demo_sheet!G10</f>
+        <v>India</v>
+      </c>
+      <c r="G10">
+        <f>demo_sheet!H10</f>
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <f>demo_sheet!I10</f>
+        <v>79</v>
+      </c>
+      <c r="I10">
+        <f>demo_sheet!J10</f>
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>